<commit_message>
add form to leads
</commit_message>
<xml_diff>
--- a/קבצי אקסל/לקוחות עסקיים.xlsx
+++ b/קבצי אקסל/לקוחות עסקיים.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y7"/>
+  <dimension ref="A1:Z9"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="1"/>
   </sheetViews>
@@ -478,6 +478,9 @@
       <c r="Y1" t="str">
         <v>דוח נתוני צריכה</v>
       </c>
+      <c r="Z1" t="str">
+        <v/>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -641,7 +644,7 @@
         <v>שלמה</v>
       </c>
       <c r="C4" t="str">
-        <v>כהן</v>
+        <v>כהןחחח</v>
       </c>
       <c r="D4" t="str">
         <v>שמעיה</v>
@@ -701,13 +704,16 @@
         <v>✔️</v>
       </c>
       <c r="W4" t="str">
-        <v>❌</v>
+        <v>✔️</v>
       </c>
       <c r="X4" t="str">
         <v>❌</v>
       </c>
       <c r="Y4" t="str">
         <v>❌</v>
+      </c>
+      <c r="Z4" t="str">
+        <v/>
       </c>
     </row>
     <row r="5">
@@ -941,9 +947,166 @@
         <v>❌</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>123456789</v>
+      </c>
+      <c r="B8" t="str">
+        <v/>
+      </c>
+      <c r="C8" t="str">
+        <v/>
+      </c>
+      <c r="D8" t="str">
+        <v>איייייי</v>
+      </c>
+      <c r="E8" t="str">
+        <v/>
+      </c>
+      <c r="F8" t="str">
+        <v/>
+      </c>
+      <c r="G8" t="str">
+        <v/>
+      </c>
+      <c r="H8" t="str">
+        <v/>
+      </c>
+      <c r="I8" t="str">
+        <v/>
+      </c>
+      <c r="J8" t="str">
+        <v/>
+      </c>
+      <c r="K8" t="str">
+        <v/>
+      </c>
+      <c r="L8" t="str">
+        <v/>
+      </c>
+      <c r="M8" t="str">
+        <v/>
+      </c>
+      <c r="N8" t="str">
+        <v/>
+      </c>
+      <c r="O8" t="str">
+        <v/>
+      </c>
+      <c r="P8" t="str">
+        <v/>
+      </c>
+      <c r="Q8" t="str">
+        <v/>
+      </c>
+      <c r="R8" t="str">
+        <v/>
+      </c>
+      <c r="S8" t="str">
+        <v/>
+      </c>
+      <c r="T8" t="str">
+        <v>❌</v>
+      </c>
+      <c r="U8" t="str">
+        <v>❌</v>
+      </c>
+      <c r="V8" t="str">
+        <v>❌</v>
+      </c>
+      <c r="W8" t="str">
+        <v>❌</v>
+      </c>
+      <c r="X8" t="str">
+        <v>❌</v>
+      </c>
+      <c r="Y8" t="str">
+        <v>❌</v>
+      </c>
+      <c r="Z8" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>111111111</v>
+      </c>
+      <c r="B9" t="str">
+        <v/>
+      </c>
+      <c r="C9" t="str">
+        <v/>
+      </c>
+      <c r="D9" t="str">
+        <v>חןןןןןן</v>
+      </c>
+      <c r="E9" t="str">
+        <v/>
+      </c>
+      <c r="F9" t="str">
+        <v/>
+      </c>
+      <c r="G9" t="str">
+        <v/>
+      </c>
+      <c r="H9" t="str">
+        <v/>
+      </c>
+      <c r="I9" t="str">
+        <v/>
+      </c>
+      <c r="J9" t="str">
+        <v/>
+      </c>
+      <c r="K9" t="str">
+        <v/>
+      </c>
+      <c r="L9" t="str">
+        <v/>
+      </c>
+      <c r="M9" t="str">
+        <v/>
+      </c>
+      <c r="N9" t="str">
+        <v/>
+      </c>
+      <c r="O9" t="str">
+        <v/>
+      </c>
+      <c r="P9" t="str">
+        <v/>
+      </c>
+      <c r="Q9" t="str">
+        <v/>
+      </c>
+      <c r="R9" t="str">
+        <v/>
+      </c>
+      <c r="S9" t="str">
+        <v/>
+      </c>
+      <c r="T9" t="str">
+        <v>❌</v>
+      </c>
+      <c r="U9" t="str">
+        <v>❌</v>
+      </c>
+      <c r="V9" t="str">
+        <v>❌</v>
+      </c>
+      <c r="W9" t="str">
+        <v>❌</v>
+      </c>
+      <c r="X9" t="str">
+        <v>❌</v>
+      </c>
+      <c r="Y9" t="str">
+        <v>❌</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:Y7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:Z9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>